<commit_message>
- Organized drivetrain class a bit.
</commit_message>
<xml_diff>
--- a/Support_Docs/DT_Calcs.xlsx
+++ b/Support_Docs/DT_Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FRC\Code\2022\X20B\X20B_2022_V1\Support_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DF451D-A96B-4D95-9430-6220ABC62A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2678ECE0-D6A6-4F70-A7E5-031A2E67B21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7ECCA170-3EBF-414F-ACF8-351CEB59FE2D}"/>
   </bookViews>
@@ -5853,8 +5853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FF2F81-024F-4828-8998-CACFEFC19902}">
   <dimension ref="A2:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6529,6 +6529,7 @@
       <c r="Q19" s="17"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C20" s="23"/>
       <c r="I20" s="21">
         <v>-15</v>
       </c>

</xml_diff>